<commit_message>
Multiplier verfication table finalized, report updated, flowchart updated
</commit_message>
<xml_diff>
--- a/assignments/soft_3/verification tests.xlsx
+++ b/assignments/soft_3/verification tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisg\Desktop\Winter 2018\CPE-233\assignments\soft_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64E5809-2EE4-4EC2-A0B6-C264F98DAA95}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9DE2B7-9B58-47F9-9D79-051798ED5659}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8040" xr2:uid="{F65589F8-EDC9-42DB-94FD-7C0E0542454D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="22">
   <si>
     <t>program 1</t>
   </si>
@@ -85,13 +85,25 @@
   </si>
   <si>
     <t>0x10</t>
+  </si>
+  <si>
+    <t>0xC1</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>12 x 1 = 12</t>
+  </si>
+  <si>
+    <t>0x0C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,13 +119,67 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -128,12 +194,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -450,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99889636-01F1-4106-8242-A39B2841EDC9}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,16 +558,16 @@
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="8" t="s">
         <v>4</v>
       </c>
     </row>
@@ -488,68 +575,85 @@
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="5">
         <v>0</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="5">
         <v>0</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="5">
         <v>4</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="5">
         <v>4</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="9" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>